<commit_message>
added NEWS, MinimumValue, MaximumValue, DOI
</commit_message>
<xml_diff>
--- a/data-raw/HarmonizedTraitDefinition.xlsx
+++ b/data-raw/HarmonizedTraitDefinition.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="169">
   <si>
     <t xml:space="preserve">Definition</t>
   </si>
@@ -34,6 +34,12 @@
     <t xml:space="preserve">Units</t>
   </si>
   <si>
+    <t xml:space="preserve">MinimumValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaximumValue</t>
+  </si>
+  <si>
     <t xml:space="preserve">Life form</t>
   </si>
   <si>
@@ -110,6 +116,12 @@
   </si>
   <si>
     <t xml:space="preserve">cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum (tree) diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dmax</t>
   </si>
   <si>
     <t xml:space="preserve">Actual plant height</t>
@@ -508,6 +520,18 @@
   </si>
   <si>
     <t xml:space="preserve">SeedLongevity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maturation height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hmat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maturation diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dmat</t>
   </si>
   <si>
     <t xml:space="preserve">Seed dry mass</t>
@@ -731,12 +755,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1022"/>
+  <dimension ref="A1:F1025"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -763,906 +787,1063 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C17" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="C20" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>55</v>
+      <c r="E23" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>64</v>
+        <v>15</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>69</v>
+      <c r="E27" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>69</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>90</v>
+        <v>15</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>90</v>
+      <c r="E41" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B44" s="3" t="s">
         <v>102</v>
       </c>
+      <c r="B44" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="C44" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>69</v>
+      <c r="E46" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>69</v>
+        <v>15</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>69</v>
+        <v>15</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>90</v>
+        <v>15</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>125</v>
+        <v>94</v>
+      </c>
+      <c r="E59" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>128</v>
+        <v>15</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B61" s="4" t="s">
         <v>130</v>
       </c>
+      <c r="B61" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="C61" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="E61" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>134</v>
+        <v>15</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E62" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B63" s="3" t="s">
         <v>136</v>
       </c>
+      <c r="B63" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="C63" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>137</v>
+        <v>15</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E63" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>34</v>
+        <v>141</v>
+      </c>
+      <c r="E64" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>26</v>
+        <v>38</v>
+      </c>
+      <c r="E65" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>144</v>
+        <v>28</v>
+      </c>
+      <c r="E66" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>147</v>
+        <v>31</v>
+      </c>
+      <c r="E67" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1673,37 +1854,48 @@
         <v>149</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>150</v>
+        <v>31</v>
+      </c>
+      <c r="E68" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C69" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>153</v>
+      <c r="E69" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C70" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" s="3"/>
+      <c r="E70" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
@@ -1713,27 +1905,70 @@
         <v>157</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E71" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>161</v>
+      </c>
+      <c r="E72" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2681,6 +2916,9 @@
     <row r="1020" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1021" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1022" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1023" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1024" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1025" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>

<commit_message>
phenology params added to harmonized
</commit_message>
<xml_diff>
--- a/data-raw/HarmonizedTraitDefinition.xlsx
+++ b/data-raw/HarmonizedTraitDefinition.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Harmonized trait definition" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Harmonized trait definition" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="196">
   <si>
     <t xml:space="preserve">Definition</t>
   </si>
@@ -589,6 +589,87 @@
   </si>
   <si>
     <t xml:space="preserve">°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaf construction costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCleaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g gluc * g dry-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sapwood construction costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCsapwood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fine root construction costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCfineroot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date to start the accumulation of degree days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t0gdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree days for leaf budburst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sgdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degrees C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base temperature for the calculation of degree days to leaf budburst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tbgdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree days corresponding to senescence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ssen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photoperiod corresponding to start counting senescence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base temperature for the calculation of degree days to senescence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tbsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discrete values, to allow for any absent/proportional/more than proportional effects of temperature  on senescence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0,1,2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discrete values, to allow for any absent/proportional/more than proportional effects of photoperiod  on senescence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ysen</t>
   </si>
 </sst>
 </file>
@@ -709,32 +790,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,17 +823,123 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F1025"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -798,10 +977,10 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3"/>
@@ -1038,7 +1217,7 @@
       <c r="A18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1086,7 +1265,7 @@
       <c r="A21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1097,7 +1276,7 @@
       <c r="A22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1114,7 +1293,7 @@
       <c r="A23" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1131,7 +1310,7 @@
       <c r="A24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1148,7 +1327,7 @@
       <c r="A25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1171,7 +1350,7 @@
       <c r="C26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E26" s="1" t="n">
@@ -1188,7 +1367,7 @@
       <c r="C27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E27" s="1" t="n">
@@ -1199,7 +1378,7 @@
       <c r="A28" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1213,7 +1392,7 @@
       <c r="A29" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -1238,7 +1417,7 @@
       <c r="A31" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1252,7 +1431,7 @@
       <c r="A32" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -1349,7 +1528,7 @@
       <c r="A38" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1363,7 +1542,7 @@
       <c r="A39" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1377,7 +1556,7 @@
       <c r="A40" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -1394,7 +1573,7 @@
       <c r="A41" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1411,7 +1590,7 @@
       <c r="A42" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -1428,7 +1607,7 @@
       <c r="A43" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -1445,7 +1624,7 @@
       <c r="A44" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -1734,7 +1913,7 @@
       <c r="C61" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="4" t="s">
         <v>132</v>
       </c>
       <c r="E61" s="1" t="n">
@@ -1745,13 +1924,13 @@
       <c r="A62" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>134</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E62" s="1" t="n">
@@ -1762,13 +1941,13 @@
       <c r="A63" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>137</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="4" t="s">
         <v>138</v>
       </c>
       <c r="E63" s="1" t="n">
@@ -1969,17 +2148,169 @@
         <v>168</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E76" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
StemEPS added to harmonized traits
</commit_message>
<xml_diff>
--- a/data-raw/HarmonizedTraitDefinition.xlsx
+++ b/data-raw/HarmonizedTraitDefinition.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="198">
   <si>
     <t xml:space="preserve">Definition</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t xml:space="preserve">LeafAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modulus of elasticity (capacity of the cell wall to resist changes in volume in response to changes in turgor) of sapwood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StemEPS</t>
   </si>
   <si>
     <t xml:space="preserve">Leaf water potential at turgor loss point</t>
@@ -934,12 +940,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1025"/>
+  <dimension ref="A1:F1026"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
+      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1423,9 +1429,7 @@
       <c r="C31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
@@ -1437,7 +1441,9 @@
       <c r="C32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
@@ -1449,19 +1455,14 @@
       <c r="C33" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>15</v>
@@ -1475,10 +1476,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>15</v>
@@ -1492,10 +1493,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>15</v>
@@ -1509,10 +1510,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>15</v>
@@ -1526,7 +1527,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>89</v>
@@ -1534,7 +1535,10 @@
       <c r="C38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="D38" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1562,25 +1566,22 @@
       <c r="C40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="E40" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="E41" s="1" t="n">
         <v>0</v>
@@ -1597,7 +1598,7 @@
         <v>15</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E42" s="1" t="n">
         <v>0</v>
@@ -1614,7 +1615,7 @@
         <v>15</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E43" s="1" t="n">
         <v>0</v>
@@ -1622,16 +1623,16 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>0</v>
@@ -1639,16 +1640,16 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E45" s="1" t="n">
         <v>0</v>
@@ -1656,16 +1657,16 @@
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E46" s="1" t="n">
         <v>0</v>
@@ -1682,18 +1683,18 @@
         <v>15</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F47" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="E47" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>15</v>
@@ -1707,10 +1708,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>15</v>
@@ -1724,22 +1725,24 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="1" t="n">
+      <c r="D50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>116</v>
@@ -1747,19 +1750,17 @@
       <c r="C51" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F51" s="1" t="n">
+      <c r="D51" s="3"/>
+      <c r="E51" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>15</v>
@@ -1773,10 +1774,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>15</v>
@@ -1790,22 +1791,24 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="1" t="n">
+      <c r="D54" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F54" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>121</v>
@@ -1813,19 +1816,17 @@
       <c r="C55" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F55" s="1" t="n">
+      <c r="D55" s="3"/>
+      <c r="E55" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>15</v>
@@ -1839,10 +1840,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>15</v>
@@ -1856,22 +1857,24 @@
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="1" t="n">
+      <c r="D58" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F58" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>126</v>
@@ -1879,9 +1882,7 @@
       <c r="C59" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="D59" s="3"/>
       <c r="E59" s="1" t="n">
         <v>0</v>
       </c>
@@ -1897,7 +1898,7 @@
         <v>15</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="E60" s="1" t="n">
         <v>0</v>
@@ -1905,50 +1906,50 @@
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="E61" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="E62" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="E63" s="1" t="n">
         <v>0</v>
@@ -1956,39 +1957,39 @@
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="C64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="E64" s="1" t="n">
         <v>0</v>
-      </c>
-      <c r="F64" s="1" t="n">
-        <v>100</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="C65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E65" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="F65" s="1" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2002,7 +2003,7 @@
         <v>15</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E66" s="1" t="n">
         <v>0</v>
@@ -2019,7 +2020,7 @@
         <v>15</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E67" s="1" t="n">
         <v>0</v>
@@ -2053,7 +2054,7 @@
         <v>15</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>152</v>
+        <v>31</v>
       </c>
       <c r="E69" s="1" t="n">
         <v>0</v>
@@ -2061,16 +2062,16 @@
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C70" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="E70" s="1" t="n">
         <v>0</v>
@@ -2078,16 +2079,16 @@
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="E71" s="1" t="n">
         <v>0</v>
@@ -2095,16 +2096,16 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="C72" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="E72" s="1" t="n">
         <v>0</v>
@@ -2112,15 +2113,20 @@
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C73" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D73" s="3"/>
+      <c r="E73" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
@@ -2144,39 +2150,34 @@
       <c r="C75" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>168</v>
-      </c>
+      <c r="D75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="C76" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E76" s="1" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="C77" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="E77" s="1" t="n">
         <v>0</v>
@@ -2193,7 +2194,7 @@
         <v>15</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E78" s="1" t="n">
         <v>0</v>
@@ -2210,35 +2211,38 @@
         <v>15</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="C80" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="C81" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2252,7 +2256,7 @@
         <v>15</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2266,21 +2270,21 @@
         <v>15</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="C84" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2294,24 +2298,37 @@
         <v>15</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="C86" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3250,6 +3267,7 @@
     <row r="1023" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1024" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1025" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1026" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>